<commit_message>
tried to solve doctor but cant
</commit_message>
<xml_diff>
--- a/sc2002/src/main/resources/Appointment.xlsx
+++ b/sc2002/src/main/resources/Appointment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>Patient ID</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>11:00</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
   </si>
 </sst>
 </file>
@@ -516,13 +513,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="12.576428571428572"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="8" width="12.576428571428572"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="9" width="16.290714285714284"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="16.290714285714284"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="22.005"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="22.005"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="8" width="12.576428571428572"/>
+    <col min="1" max="1" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -721,7 +718,7 @@
         <v>21</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">

</xml_diff>

<commit_message>
Touched up abit of formatting
</commit_message>
<xml_diff>
--- a/sc2002/src/main/resources/Appointment.xlsx
+++ b/sc2002/src/main/resources/Appointment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>Patient ID</t>
   </si>
@@ -97,10 +97,10 @@
     <t>Confirmed</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>29/10/2024</t>
+  </si>
+  <si>
+    <t>Declined</t>
   </si>
 </sst>
 </file>
@@ -108,7 +108,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +140,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri (Body)"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -185,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -206,6 +212,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -525,13 +537,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="8" width="12.576428571428572"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="8" width="12.576428571428572"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="9" width="16.290714285714284"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="8" width="16.290714285714284"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="10" width="22.005"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="10" width="22.005"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="8" width="12.576428571428572"/>
+    <col min="1" max="1" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="22.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -781,27 +793,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s" s="8">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s" s="8">
+      <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="n" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="D12" t="s" s="8">
+      <c r="C12" s="8">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E12" t="s" s="10">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s" s="10">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s" s="8">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>